<commit_message>
Issue with deletion of bots solved
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,114 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\learn_coding\Selenium\Insta_Bot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270CAC88-6FF5-47B8-8E74-DC7D900B854E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Account-Daten" sheetId="1" r:id="rId1"/>
-    <sheet name="Bots" sheetId="2" r:id="rId2"/>
+    <sheet name="Account-Daten" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bots" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Passwort</t>
-  </si>
-  <si>
-    <t>Email-Adresse</t>
-  </si>
-  <si>
-    <t>hans.peter.der.echte</t>
-  </si>
-  <si>
-    <t>test.python</t>
-  </si>
-  <si>
-    <t>test.mail.trichter@gmail.com</t>
-  </si>
-  <si>
-    <t>Doublixah</t>
-  </si>
-  <si>
-    <t>Candicejokenotfunny420</t>
-  </si>
-  <si>
-    <t>checkmeout1337</t>
-  </si>
-  <si>
-    <t>41KKIZ6h8JReWyxzlkSL</t>
-  </si>
-  <si>
-    <t>checkmeout1337@gmail.com</t>
-  </si>
-  <si>
-    <t>relextending</t>
-  </si>
-  <si>
-    <t>rgs_ide</t>
-  </si>
-  <si>
-    <t>vince.skl</t>
-  </si>
-  <si>
-    <t>dertrichter_jr</t>
-  </si>
-  <si>
-    <t>renaldo_3h</t>
-  </si>
-  <si>
-    <t>j_a_n._</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -270,58 +209,139 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -621,182 +641,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="12" customWidth="1"/>
+    <col width="34.140625" customWidth="1" style="12" min="1" max="1"/>
+    <col width="22.7109375" customWidth="1" style="4" min="2" max="2"/>
+    <col width="34.42578125" customWidth="1" style="12" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>5</v>
+    <row r="1" ht="15.75" customHeight="1" s="12" thickBot="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Passwort</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Email-Adresse</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="12" thickTop="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hans.peter.der.echte</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>test.mail.trichter@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Doublixah</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>test.mail.trichter@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Candicejokenotfunny420</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>test.mail.trichter@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>checkmeout1337</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>41KKIZ6h8JReWyxzlkSL</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>relextending</t>
+        </is>
+      </c>
+      <c r="B6" s="18" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C6" s="18" t="inlineStr">
+        <is>
+          <t>test.mail.trichter@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rgs_ide</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t>test.mail.trichter@gmail.com</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" style="12" customWidth="1"/>
+    <col width="30.7109375" customWidth="1" style="12" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>16</v>
+    <row r="1" ht="15.75" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>hans.peter.der.echte</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Doublixah</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Candicejokenotfunny420</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>checkmeout1337</t>
+        </is>
+      </c>
+      <c r="E1" s="19" t="inlineStr">
+        <is>
+          <t>relextending</t>
+        </is>
+      </c>
+      <c r="F1" s="21" t="inlineStr">
+        <is>
+          <t>rgs_ide</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="12" thickTop="1">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>vince.skl</t>
+        </is>
+      </c>
+      <c r="B2" s="15" t="inlineStr">
+        <is>
+          <t>vince.skl</t>
+        </is>
+      </c>
+      <c r="C2" s="15" t="inlineStr">
+        <is>
+          <t>vince.skl</t>
+        </is>
+      </c>
+      <c r="D2" s="16" t="inlineStr">
+        <is>
+          <t>vince.skl</t>
+        </is>
+      </c>
+      <c r="E2" s="22" t="inlineStr">
+        <is>
+          <t>vince.skl</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
+      <c r="D3" s="16" t="inlineStr">
+        <is>
+          <t>renaldo_3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="inlineStr">
+        <is>
+          <t>renaldo_3h</t>
+        </is>
+      </c>
+      <c r="D4" s="17" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14" t="inlineStr">
+        <is>
+          <t>j_a_n._</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new commenting system
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,53 +1,166 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\learn_coding\Selenium\Insta_Bot\Code\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EACD92-F577-48F2-A441-8AE81FABA41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Account-Daten" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bots" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Account-Daten" sheetId="1" r:id="rId1"/>
+    <sheet name="Bots" sheetId="2" r:id="rId2"/>
+    <sheet name="Comments" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Passwort</t>
+  </si>
+  <si>
+    <t>Email-Adresse</t>
+  </si>
+  <si>
+    <t>hans.peter.der.echte</t>
+  </si>
+  <si>
+    <t>test.python</t>
+  </si>
+  <si>
+    <t>test.mail.trichter@gmail.com</t>
+  </si>
+  <si>
+    <t>Doublixah</t>
+  </si>
+  <si>
+    <t>Candicejokenotfunny420</t>
+  </si>
+  <si>
+    <t>checkmeout1337</t>
+  </si>
+  <si>
+    <t>41KKIZ6h8JReWyxzlkSL</t>
+  </si>
+  <si>
+    <t>checkmeout1337@gmail.com</t>
+  </si>
+  <si>
+    <t>relextending</t>
+  </si>
+  <si>
+    <t>rgs_ide</t>
+  </si>
+  <si>
+    <t>vince.skl</t>
+  </si>
+  <si>
+    <t>beste_jodel</t>
+  </si>
+  <si>
+    <t>dertrichter_jr</t>
+  </si>
+  <si>
+    <t>renaldo_3h</t>
+  </si>
+  <si>
+    <t>montanablack</t>
+  </si>
+  <si>
+    <t>j_a_n._</t>
+  </si>
+  <si>
+    <t>Cooler Typ</t>
+  </si>
+  <si>
+    <t>Sehr stark</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Maschine</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>Du beast</t>
+  </si>
+  <si>
+    <t>Beast</t>
+  </si>
+  <si>
+    <t>Stark bro</t>
+  </si>
+  <si>
+    <t>Stabil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>aha lul</t>
+  </si>
+  <si>
+    <t>bertha</t>
+  </si>
+  <si>
+    <t>uwe</t>
+  </si>
+  <si>
+    <t>get it</t>
+  </si>
+  <si>
+    <t>ready</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -221,119 +334,77 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick"/>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -633,268 +704,282 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="34.140625" customWidth="1" style="12" min="1" max="1"/>
-    <col width="22.7109375" customWidth="1" style="4" min="2" max="2"/>
-    <col width="34.42578125" customWidth="1" style="12" min="3" max="3"/>
+    <col min="1" max="1" width="34.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="12" thickBot="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Passwort</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Email-Adresse</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="12" thickTop="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>hans.peter.der.echte</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>test.python</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>test.mail.trichter@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Doublixah</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>test.python</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>test.mail.trichter@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Candicejokenotfunny420</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>test.python</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>test.mail.trichter@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>checkmeout1337</t>
-        </is>
-      </c>
-      <c r="B5" s="7" t="inlineStr">
-        <is>
-          <t>41KKIZ6h8JReWyxzlkSL</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="inlineStr">
-        <is>
-          <t>checkmeout1337@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>relextending</t>
-        </is>
-      </c>
-      <c r="B6" s="18" t="inlineStr">
-        <is>
-          <t>test.python</t>
-        </is>
-      </c>
-      <c r="C6" s="18" t="inlineStr">
-        <is>
-          <t>test.mail.trichter@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>rgs_ide</t>
-        </is>
-      </c>
-      <c r="B7" s="20" t="inlineStr">
-        <is>
-          <t>test.python</t>
-        </is>
-      </c>
-      <c r="C7" s="20" t="inlineStr">
-        <is>
-          <t>test.mail.trichter@gmail.com</t>
-        </is>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="30.7109375" customWidth="1" style="12" min="2" max="2"/>
+    <col min="2" max="2" width="30.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A1" s="9" t="inlineStr">
-        <is>
-          <t>hans.peter.der.echte</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Doublixah</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Candicejokenotfunny420</t>
-        </is>
-      </c>
-      <c r="D1" s="11" t="inlineStr">
-        <is>
-          <t>checkmeout1337</t>
-        </is>
-      </c>
-      <c r="E1" s="19" t="inlineStr">
-        <is>
-          <t>relextending</t>
-        </is>
-      </c>
-      <c r="F1" s="21" t="inlineStr">
-        <is>
-          <t>rgs_ide</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="12" thickTop="1">
-      <c r="A2" s="8" t="inlineStr">
-        <is>
-          <t>vince.skl</t>
-        </is>
-      </c>
-      <c r="B2" s="15" t="inlineStr">
-        <is>
-          <t>vince.skl</t>
-        </is>
-      </c>
-      <c r="C2" s="15" t="inlineStr">
-        <is>
-          <t>vince.skl</t>
-        </is>
-      </c>
-      <c r="D2" s="16" t="inlineStr">
-        <is>
-          <t>vince.skl</t>
-        </is>
-      </c>
-      <c r="E2" s="22" t="inlineStr">
-        <is>
-          <t>vince.skl</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="inlineStr">
-        <is>
-          <t>dertrichter_jr</t>
-        </is>
-      </c>
-      <c r="B3" s="17" t="inlineStr">
-        <is>
-          <t>dertrichter_jr</t>
-        </is>
-      </c>
-      <c r="C3" s="17" t="inlineStr">
-        <is>
-          <t>dertrichter_jr</t>
-        </is>
-      </c>
-      <c r="D3" s="16" t="inlineStr">
-        <is>
-          <t>renaldo_3h</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="14" t="inlineStr">
-        <is>
-          <t>renaldo_3h</t>
-        </is>
-      </c>
-      <c r="D4" s="24" t="inlineStr">
-        <is>
-          <t>dertrichter_jr</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="14" t="inlineStr">
-        <is>
-          <t>j_a_n._</t>
-        </is>
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ka hab eigentlich nix geändert
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -804,7 +804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -949,9 +949,21 @@
           <t>beste_jodel</t>
         </is>
       </c>
+      <c r="C5" s="27" t="inlineStr">
+        <is>
+          <t>harry styles</t>
+        </is>
+      </c>
       <c r="E5" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" s="27" t="inlineStr">
+        <is>
+          <t>harry styles</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bugs related to multiprocessing Added a new liking function to ensure that videos can also be liked
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -812,7 +812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -1026,6 +1026,11 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="C7" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
       <c r="D7" s="26" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1053,6 +1058,11 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="C8" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
       <c r="D8" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1080,6 +1090,11 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="C9" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
       <c r="D9" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1088,6 +1103,11 @@
       <c r="E9" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
         </is>
       </c>
     </row>
@@ -1097,6 +1117,16 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="B10" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="C10" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
       <c r="D10" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1107,25 +1137,231 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="F10" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
     </row>
     <row r="11">
+      <c r="A11" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B11" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="C11" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
       <c r="D11" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="E11" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="F11" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
     </row>
     <row r="12">
+      <c r="A12" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B12" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="C12" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
       <c r="D12" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="E12" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="F12" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
     </row>
     <row r="13">
+      <c r="A13" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B13" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
       <c r="D13" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="E13" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="F13" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B14" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="D14" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="E14" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="F14" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B15" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="D15" s="27" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="E15" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B16" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="D16" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="E16" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="B17" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="D17" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="E17" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="D18" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+      <c r="E18" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="27" t="inlineStr">
+        <is>
+          <t>nbl</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Connected the GUI to the bot program + improvement of the bot
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2160" yWindow="0" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account-Daten" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Bots" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="name" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -47,7 +48,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -245,6 +246,44 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -254,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -291,6 +330,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -668,10 +711,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -757,7 +800,7 @@
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>41KKIZ6h8JReWyxzlkSL</t>
+          <t>test.python</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
@@ -797,6 +840,91 @@
       <c r="C7" s="20" t="inlineStr">
         <is>
           <t>test.mail.trichter@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>paul.squeeky</t>
+        </is>
+      </c>
+      <c r="B8" s="28" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C8" s="28" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>N2S.universe</t>
+        </is>
+      </c>
+      <c r="B9" s="28" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C9" s="28" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dtrmnd_42</t>
+        </is>
+      </c>
+      <c r="B10" s="28" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C10" s="28" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>troy.bt</t>
+        </is>
+      </c>
+      <c r="B11" s="28" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C11" s="28" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CodingIsFun2021</t>
+        </is>
+      </c>
+      <c r="B12" s="28" t="inlineStr">
+        <is>
+          <t>test.python</t>
+        </is>
+      </c>
+      <c r="C12" s="28" t="inlineStr">
+        <is>
+          <t>checkmeout1337@gmail.com</t>
         </is>
       </c>
     </row>
@@ -812,9 +940,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -854,6 +982,31 @@
           <t>rgs_ide</t>
         </is>
       </c>
+      <c r="G1" s="29" t="inlineStr">
+        <is>
+          <t>paul.squeeky</t>
+        </is>
+      </c>
+      <c r="H1" s="29" t="inlineStr">
+        <is>
+          <t>N2S.universe</t>
+        </is>
+      </c>
+      <c r="I1" s="29" t="inlineStr">
+        <is>
+          <t>dtrmnd_42</t>
+        </is>
+      </c>
+      <c r="J1" s="29" t="inlineStr">
+        <is>
+          <t>troy.bt</t>
+        </is>
+      </c>
+      <c r="K1" s="29" t="inlineStr">
+        <is>
+          <t>CodingIsFun2021</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="12" thickTop="1">
       <c r="A2" s="8" t="inlineStr">
@@ -886,6 +1039,26 @@
           <t>beste_jodel</t>
         </is>
       </c>
+      <c r="G2" s="31" t="inlineStr">
+        <is>
+          <t>vinc.skl</t>
+        </is>
+      </c>
+      <c r="H2" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
+      <c r="I2" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="J2" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -918,6 +1091,11 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="I3" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="inlineStr">
@@ -950,6 +1128,11 @@
           <t>trichterdraws</t>
         </is>
       </c>
+      <c r="I4" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="14" t="inlineStr">
@@ -1218,6 +1401,11 @@
           <t>nbl</t>
         </is>
       </c>
+      <c r="C13" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
       <c r="D13" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1245,6 +1433,11 @@
           <t>nbl</t>
         </is>
       </c>
+      <c r="C14" s="31" t="inlineStr">
+        <is>
+          <t>nba</t>
+        </is>
+      </c>
       <c r="D14" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1272,6 +1465,11 @@
           <t>nbl</t>
         </is>
       </c>
+      <c r="C15" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
       <c r="D15" s="27" t="inlineStr">
         <is>
           <t>trichterdraws</t>
@@ -1280,6 +1478,11 @@
       <c r="E15" s="27" t="inlineStr">
         <is>
           <t>nbl</t>
+        </is>
+      </c>
+      <c r="F15" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
         </is>
       </c>
     </row>
@@ -1304,6 +1507,11 @@
           <t>nbl</t>
         </is>
       </c>
+      <c r="F16" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="27" t="inlineStr">
@@ -1333,6 +1541,11 @@
           <t>nbl</t>
         </is>
       </c>
+      <c r="B18" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
       <c r="D18" s="27" t="inlineStr">
         <is>
           <t>nbl</t>
@@ -1345,6 +1558,21 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
+      <c r="B19" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+      <c r="D19" s="31" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
           <t>nbl</t>
@@ -1352,6 +1580,16 @@
       </c>
     </row>
     <row r="20">
+      <c r="B20" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
+      <c r="D20" s="31" t="inlineStr">
+        <is>
+          <t>dertrichter_jr</t>
+        </is>
+      </c>
       <c r="E20" s="27" t="inlineStr">
         <is>
           <t>nbl</t>
@@ -1362,6 +1600,41 @@
       <c r="E21" s="27" t="inlineStr">
         <is>
           <t>nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" s="31" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" s="31" t="inlineStr">
+        <is>
+          <t>trichterdraws</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" s="31" t="inlineStr">
+        <is>
+          <t>vince_skl</t>
         </is>
       </c>
     </row>
@@ -1369,4 +1642,287 @@
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="30" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="30" t="inlineStr">
+        <is>
+          <t>word</t>
+        </is>
+      </c>
+      <c r="C1" s="30" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="D1" s="30" t="inlineStr">
+        <is>
+          <t>seperator</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>peter</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>universe</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>justin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>paul</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>coding</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>clarence</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hacking</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>larry</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>cool</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>kevin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>theswagger</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>henry</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>inferno</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>nico</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>murphy</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>pro</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>cooper</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>gamer</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>claire</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>drawing</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dalton</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>fit</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>finn</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>elias</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>gaming</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>will</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>jay</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>bruce</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>